<commit_message>
use snaking algorithm rather than recursive + update player data
</commit_message>
<xml_diff>
--- a/player_data.xlsx
+++ b/player_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingqi/Desktop/teampartition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846CB568-BD5A-914C-B9B9-4B299653B42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A9139E-006C-0643-BBB9-D97B909F3269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27980" windowHeight="18380" xr2:uid="{8F58AEF8-0A0C-344B-AB88-3ED362C15D30}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="66">
   <si>
     <t>Setter</t>
   </si>
@@ -1005,12 +1005,6 @@
       <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
       <c r="I14" t="s">
         <v>10</v>
       </c>
@@ -1065,10 +1059,10 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" t="s">
         <v>10</v>
@@ -1186,6 +1180,9 @@
         <v>10</v>
       </c>
       <c r="J20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1358,7 +1355,7 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1377,7 +1374,7 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
@@ -1455,10 +1452,10 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J31" t="s">
         <v>44</v>
@@ -1798,13 +1795,10 @@
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
-      </c>
-      <c r="I44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -1885,7 +1879,7 @@
     <sortCondition ref="C2:C47"/>
     <sortCondition ref="B2:B47"/>
   </sortState>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K1048576" xr:uid="{7C74D076-EA55-1047-A177-90DE1DE45E39}">
       <formula1>$A:$A</formula1>
     </dataValidation>

</xml_diff>